<commit_message>
added changes to database upload so that sequence aligns
</commit_message>
<xml_diff>
--- a/database/Project_Data.xlsx
+++ b/database/Project_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffb\Desktop\Tecky\WSP\WSP012_Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B507C17F-604F-478E-9282-B70C9DA5DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4331CFE3-B876-4A94-ADFC-AE89FD0E1815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19042" yWindow="-1103" windowWidth="19125" windowHeight="11236" firstSheet="9" activeTab="13" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1089">
   <si>
     <t>id</t>
   </si>
@@ -3306,6 +3306,12 @@
   </si>
   <si>
     <t>2023-01-18 14:55:47</t>
+  </si>
+  <si>
+    <t>38806715</t>
+  </si>
+  <si>
+    <t>$2a$04$AvIPbbagfXqklLVaXXYiZ.xHYIDmL.xvvd.UrHySr5k4AEaaNH/82</t>
   </si>
 </sst>
 </file>
@@ -3721,8 +3727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89681126-5237-455A-856C-2B26CBD7FB95}">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="R89" sqref="R89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3733,7 +3739,7 @@
     <col min="4" max="4" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
@@ -3792,7 +3798,7 @@
         <v>24525402</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -3824,7 +3830,7 @@
         <v>57060794</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -3856,7 +3862,7 @@
         <v>94713906</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
@@ -3888,7 +3894,7 @@
         <v>14685757</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H5" s="1">
         <v>2</v>
@@ -3920,7 +3926,7 @@
         <v>60515705</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -3952,7 +3958,7 @@
         <v>28207629</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -3984,7 +3990,7 @@
         <v>52947240</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -4016,7 +4022,7 @@
         <v>34170541</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
@@ -4048,7 +4054,7 @@
         <v>82903004</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H10" s="1">
         <v>2</v>
@@ -4080,7 +4086,7 @@
         <v>60303237</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -4112,7 +4118,7 @@
         <v>36493531</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
@@ -4144,7 +4150,7 @@
         <v>82</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H13" s="1">
         <v>2</v>
@@ -4176,7 +4182,7 @@
         <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H14" s="1">
         <v>2</v>
@@ -4208,7 +4214,7 @@
         <v>46626259</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H15" s="1">
         <v>2</v>
@@ -4240,7 +4246,7 @@
         <v>14903335</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H16" s="1">
         <v>2</v>
@@ -4272,7 +4278,7 @@
         <v>86583052</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -4304,7 +4310,7 @@
         <v>69011866</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H18" s="1">
         <v>2</v>
@@ -4336,7 +4342,7 @@
         <v>86467584</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
@@ -4368,7 +4374,7 @@
         <v>84</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H20" s="1">
         <v>2</v>
@@ -4400,7 +4406,7 @@
         <v>38142143</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H21" s="1">
         <v>2</v>
@@ -4432,7 +4438,7 @@
         <v>62084515</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -4464,7 +4470,7 @@
         <v>25890369</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H23" s="1">
         <v>2</v>
@@ -4496,7 +4502,7 @@
         <v>10223266</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H24" s="1">
         <v>2</v>
@@ -4528,7 +4534,7 @@
         <v>21984532</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H25" s="1">
         <v>2</v>
@@ -4560,7 +4566,7 @@
         <v>37299097</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H26" s="1">
         <v>2</v>
@@ -4592,7 +4598,7 @@
         <v>42689302</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H27" s="1">
         <v>2</v>
@@ -4624,7 +4630,7 @@
         <v>92825467</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H28" s="1">
         <v>2</v>
@@ -4656,7 +4662,7 @@
         <v>59809431</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H29" s="1">
         <v>2</v>
@@ -4688,7 +4694,7 @@
         <v>90994799</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H30" s="1">
         <v>2</v>
@@ -4720,7 +4726,7 @@
         <v>92235387</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H31" s="1">
         <v>2</v>
@@ -4752,7 +4758,7 @@
         <v>79262859</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H32" s="1">
         <v>2</v>
@@ -4784,7 +4790,7 @@
         <v>85</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H33" s="1">
         <v>2</v>
@@ -4816,7 +4822,7 @@
         <v>26434632</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H34" s="1">
         <v>2</v>
@@ -4848,7 +4854,7 @@
         <v>78887454</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H35" s="1">
         <v>2</v>
@@ -4880,7 +4886,7 @@
         <v>72440777</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H36" s="1">
         <v>2</v>
@@ -4912,7 +4918,7 @@
         <v>86</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H37" s="1">
         <v>1</v>
@@ -4944,7 +4950,7 @@
         <v>19091891</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H38" s="1">
         <v>2</v>
@@ -4976,7 +4982,7 @@
         <v>90557839</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H39" s="1">
         <v>2</v>
@@ -5008,7 +5014,7 @@
         <v>68043701</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H40" s="1">
         <v>2</v>
@@ -5040,7 +5046,7 @@
         <v>42426903</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H41" s="1">
         <v>2</v>
@@ -5072,7 +5078,7 @@
         <v>46681742</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H42" s="1">
         <v>2</v>
@@ -5104,7 +5110,7 @@
         <v>93975858</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H43" s="1">
         <v>2</v>
@@ -5136,7 +5142,7 @@
         <v>35188903</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H44" s="1">
         <v>2</v>
@@ -5168,7 +5174,7 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H45" s="1">
         <v>2</v>
@@ -5200,7 +5206,7 @@
         <v>28729013</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H46" s="1">
         <v>1</v>
@@ -5232,7 +5238,7 @@
         <v>22570600</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H47" s="1">
         <v>2</v>
@@ -5264,7 +5270,7 @@
         <v>88</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H48" s="1">
         <v>2</v>
@@ -5296,7 +5302,7 @@
         <v>86922958</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H49" s="1">
         <v>2</v>
@@ -5328,7 +5334,7 @@
         <v>86436566</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H50" s="1">
         <v>2</v>
@@ -5360,7 +5366,7 @@
         <v>75380206</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H51" s="1">
         <v>2</v>
@@ -5392,7 +5398,7 @@
         <v>18270909</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H52" s="1">
         <v>2</v>
@@ -5424,7 +5430,7 @@
         <v>62564319</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H53" s="1">
         <v>2</v>
@@ -5456,7 +5462,7 @@
         <v>73182935</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H54" s="1">
         <v>2</v>
@@ -5488,7 +5494,7 @@
         <v>21770892</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H55" s="1">
         <v>2</v>
@@ -5520,7 +5526,7 @@
         <v>89032776</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H56" s="1">
         <v>2</v>
@@ -5552,7 +5558,7 @@
         <v>84401453</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H57" s="1">
         <v>2</v>
@@ -5584,7 +5590,7 @@
         <v>34287307</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H58" s="1">
         <v>1</v>
@@ -5616,7 +5622,7 @@
         <v>18713246</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H59" s="1">
         <v>2</v>
@@ -5648,7 +5654,7 @@
         <v>55298168</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H60" s="1">
         <v>2</v>
@@ -5680,7 +5686,7 @@
         <v>31430907</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H61" s="1">
         <v>2</v>
@@ -5712,7 +5718,7 @@
         <v>47024498</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H62" s="1">
         <v>2</v>
@@ -5744,7 +5750,7 @@
         <v>89</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H63" s="1">
         <v>2</v>
@@ -5776,7 +5782,7 @@
         <v>17040135</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H64" s="1">
         <v>2</v>
@@ -5808,7 +5814,7 @@
         <v>68540910</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H65" s="1">
         <v>2</v>
@@ -5840,7 +5846,7 @@
         <v>80325877</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H66" s="1">
         <v>2</v>
@@ -5872,7 +5878,7 @@
         <v>67307935</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H67" s="1">
         <v>2</v>
@@ -5904,7 +5910,7 @@
         <v>19534338</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H68" s="1">
         <v>2</v>
@@ -5936,7 +5942,7 @@
         <v>89258111</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H69" s="1">
         <v>2</v>
@@ -5968,7 +5974,7 @@
         <v>29486020</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H70" s="1">
         <v>1</v>
@@ -6000,7 +6006,7 @@
         <v>30534151</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H71" s="1">
         <v>2</v>
@@ -6032,7 +6038,7 @@
         <v>40492520</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H72" s="1">
         <v>2</v>
@@ -6064,7 +6070,7 @@
         <v>40672045</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H73" s="1">
         <v>2</v>
@@ -6096,7 +6102,7 @@
         <v>46464032</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H74" s="1">
         <v>2</v>
@@ -6128,7 +6134,7 @@
         <v>49376026</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H75" s="1">
         <v>2</v>
@@ -6160,7 +6166,7 @@
         <v>73075459</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H76" s="1">
         <v>2</v>
@@ -6192,7 +6198,7 @@
         <v>98052346</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H77" s="1">
         <v>1</v>
@@ -6224,7 +6230,7 @@
         <v>15481084</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H78" s="1">
         <v>2</v>
@@ -6256,7 +6262,7 @@
         <v>39630579</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H79" s="1">
         <v>2</v>
@@ -6288,7 +6294,7 @@
         <v>83146202</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H80" s="1">
         <v>2</v>
@@ -6320,7 +6326,7 @@
         <v>86707179</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H81" s="1">
         <v>2</v>
@@ -6352,7 +6358,7 @@
         <v>40342542</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H82" s="1">
         <v>1</v>
@@ -6384,7 +6390,7 @@
         <v>78791420</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H83" s="1">
         <v>2</v>
@@ -6412,11 +6418,11 @@
       <c r="D84" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E84" s="1">
-        <v>38806715</v>
+      <c r="E84" s="1" t="s">
+        <v>1087</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H84" s="1">
         <v>2</v>
@@ -6448,7 +6454,7 @@
         <v>92040568</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H85" s="1">
         <v>2</v>
@@ -6480,7 +6486,7 @@
         <v>90</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H86" s="1">
         <v>2</v>
@@ -6512,7 +6518,7 @@
         <v>81700104</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H87" s="1">
         <v>1</v>
@@ -6544,7 +6550,7 @@
         <v>78771117</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H88" s="1">
         <v>2</v>
@@ -6576,7 +6582,7 @@
         <v>92</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H89" s="1">
         <v>2</v>
@@ -6608,7 +6614,7 @@
         <v>93</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H90" s="1">
         <v>2</v>
@@ -6640,7 +6646,7 @@
         <v>24460781</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H91" s="1">
         <v>1</v>
@@ -6672,7 +6678,7 @@
         <v>38447660</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H92" s="1">
         <v>2</v>
@@ -6704,7 +6710,7 @@
         <v>91</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H93" s="1">
         <v>2</v>
@@ -6736,7 +6742,7 @@
         <v>62104183</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H94" s="1">
         <v>2</v>
@@ -6768,7 +6774,7 @@
         <v>54709573</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H95" s="1">
         <v>2</v>
@@ -6800,7 +6806,7 @@
         <v>84352829</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H96" s="1">
         <v>2</v>
@@ -6832,7 +6838,7 @@
         <v>72641669</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H97" s="1">
         <v>1</v>
@@ -6864,7 +6870,7 @@
         <v>77424584</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H98" s="1">
         <v>2</v>
@@ -6896,7 +6902,7 @@
         <v>11627771</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H99" s="1">
         <v>2</v>
@@ -6928,7 +6934,7 @@
         <v>17389523</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H100" s="1">
         <v>2</v>
@@ -6960,7 +6966,7 @@
         <v>24800409</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>6</v>
+        <v>1088</v>
       </c>
       <c r="H101" s="1">
         <v>2</v>
@@ -7756,7 +7762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1411D3-6099-4529-BBF2-121DB70152D1}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated the database so it finally works, created upload
</commit_message>
<xml_diff>
--- a/database/Project_Data.xlsx
+++ b/database/Project_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffb\Desktop\Tecky\WSP\WSP012_Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4331CFE3-B876-4A94-ADFC-AE89FD0E1815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B2C645-E5FF-4C28-A5BC-134CAB3AFEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
+    <workbookView xWindow="375" yWindow="240" windowWidth="19005" windowHeight="11175" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1088">
   <si>
     <t>id</t>
   </si>
@@ -3309,9 +3309,6 @@
   </si>
   <si>
     <t>38806715</t>
-  </si>
-  <si>
-    <t>$2a$04$AvIPbbagfXqklLVaXXYiZ.xHYIDmL.xvvd.UrHySr5k4AEaaNH/82</t>
   </si>
 </sst>
 </file>
@@ -3727,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89681126-5237-455A-856C-2B26CBD7FB95}">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="R89" sqref="R89"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,7 +3795,7 @@
         <v>24525402</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -3830,7 +3827,7 @@
         <v>57060794</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -3862,7 +3859,7 @@
         <v>94713906</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
@@ -3894,7 +3891,7 @@
         <v>14685757</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1">
         <v>2</v>
@@ -3926,7 +3923,7 @@
         <v>60515705</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -3958,7 +3955,7 @@
         <v>28207629</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -3990,7 +3987,7 @@
         <v>52947240</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -4022,7 +4019,7 @@
         <v>34170541</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
@@ -4054,7 +4051,7 @@
         <v>82903004</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1">
         <v>2</v>
@@ -4086,7 +4083,7 @@
         <v>60303237</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -4118,7 +4115,7 @@
         <v>36493531</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
@@ -4150,7 +4147,7 @@
         <v>82</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1">
         <v>2</v>
@@ -4182,7 +4179,7 @@
         <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H14" s="1">
         <v>2</v>
@@ -4214,7 +4211,7 @@
         <v>46626259</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H15" s="1">
         <v>2</v>
@@ -4246,7 +4243,7 @@
         <v>14903335</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H16" s="1">
         <v>2</v>
@@ -4278,7 +4275,7 @@
         <v>86583052</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -4310,7 +4307,7 @@
         <v>69011866</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H18" s="1">
         <v>2</v>
@@ -4342,7 +4339,7 @@
         <v>86467584</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H19" s="1">
         <v>2</v>
@@ -4374,7 +4371,7 @@
         <v>84</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H20" s="1">
         <v>2</v>
@@ -4406,7 +4403,7 @@
         <v>38142143</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H21" s="1">
         <v>2</v>
@@ -4438,7 +4435,7 @@
         <v>62084515</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -4470,7 +4467,7 @@
         <v>25890369</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H23" s="1">
         <v>2</v>
@@ -4502,7 +4499,7 @@
         <v>10223266</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H24" s="1">
         <v>2</v>
@@ -4534,7 +4531,7 @@
         <v>21984532</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H25" s="1">
         <v>2</v>
@@ -4566,7 +4563,7 @@
         <v>37299097</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H26" s="1">
         <v>2</v>
@@ -4598,7 +4595,7 @@
         <v>42689302</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H27" s="1">
         <v>2</v>
@@ -4630,7 +4627,7 @@
         <v>92825467</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H28" s="1">
         <v>2</v>
@@ -4662,7 +4659,7 @@
         <v>59809431</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H29" s="1">
         <v>2</v>
@@ -4694,7 +4691,7 @@
         <v>90994799</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H30" s="1">
         <v>2</v>
@@ -4726,7 +4723,7 @@
         <v>92235387</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H31" s="1">
         <v>2</v>
@@ -4758,7 +4755,7 @@
         <v>79262859</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H32" s="1">
         <v>2</v>
@@ -4790,7 +4787,7 @@
         <v>85</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H33" s="1">
         <v>2</v>
@@ -4822,7 +4819,7 @@
         <v>26434632</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H34" s="1">
         <v>2</v>
@@ -4854,7 +4851,7 @@
         <v>78887454</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H35" s="1">
         <v>2</v>
@@ -4886,7 +4883,7 @@
         <v>72440777</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H36" s="1">
         <v>2</v>
@@ -4918,7 +4915,7 @@
         <v>86</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H37" s="1">
         <v>1</v>
@@ -4950,7 +4947,7 @@
         <v>19091891</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H38" s="1">
         <v>2</v>
@@ -4982,7 +4979,7 @@
         <v>90557839</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H39" s="1">
         <v>2</v>
@@ -5014,7 +5011,7 @@
         <v>68043701</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H40" s="1">
         <v>2</v>
@@ -5046,7 +5043,7 @@
         <v>42426903</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H41" s="1">
         <v>2</v>
@@ -5078,7 +5075,7 @@
         <v>46681742</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H42" s="1">
         <v>2</v>
@@ -5110,7 +5107,7 @@
         <v>93975858</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H43" s="1">
         <v>2</v>
@@ -5142,7 +5139,7 @@
         <v>35188903</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H44" s="1">
         <v>2</v>
@@ -5174,7 +5171,7 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H45" s="1">
         <v>2</v>
@@ -5206,7 +5203,7 @@
         <v>28729013</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H46" s="1">
         <v>1</v>
@@ -5238,7 +5235,7 @@
         <v>22570600</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H47" s="1">
         <v>2</v>
@@ -5270,7 +5267,7 @@
         <v>88</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H48" s="1">
         <v>2</v>
@@ -5302,7 +5299,7 @@
         <v>86922958</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H49" s="1">
         <v>2</v>
@@ -5334,7 +5331,7 @@
         <v>86436566</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H50" s="1">
         <v>2</v>
@@ -5366,7 +5363,7 @@
         <v>75380206</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H51" s="1">
         <v>2</v>
@@ -5398,7 +5395,7 @@
         <v>18270909</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H52" s="1">
         <v>2</v>
@@ -5430,7 +5427,7 @@
         <v>62564319</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H53" s="1">
         <v>2</v>
@@ -5462,7 +5459,7 @@
         <v>73182935</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H54" s="1">
         <v>2</v>
@@ -5494,7 +5491,7 @@
         <v>21770892</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H55" s="1">
         <v>2</v>
@@ -5526,7 +5523,7 @@
         <v>89032776</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H56" s="1">
         <v>2</v>
@@ -5558,7 +5555,7 @@
         <v>84401453</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H57" s="1">
         <v>2</v>
@@ -5590,7 +5587,7 @@
         <v>34287307</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H58" s="1">
         <v>1</v>
@@ -5622,7 +5619,7 @@
         <v>18713246</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H59" s="1">
         <v>2</v>
@@ -5654,7 +5651,7 @@
         <v>55298168</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H60" s="1">
         <v>2</v>
@@ -5686,7 +5683,7 @@
         <v>31430907</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H61" s="1">
         <v>2</v>
@@ -5718,7 +5715,7 @@
         <v>47024498</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H62" s="1">
         <v>2</v>
@@ -5750,7 +5747,7 @@
         <v>89</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H63" s="1">
         <v>2</v>
@@ -5782,7 +5779,7 @@
         <v>17040135</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H64" s="1">
         <v>2</v>
@@ -5814,7 +5811,7 @@
         <v>68540910</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H65" s="1">
         <v>2</v>
@@ -5846,7 +5843,7 @@
         <v>80325877</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H66" s="1">
         <v>2</v>
@@ -5878,7 +5875,7 @@
         <v>67307935</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H67" s="1">
         <v>2</v>
@@ -5910,7 +5907,7 @@
         <v>19534338</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H68" s="1">
         <v>2</v>
@@ -5942,7 +5939,7 @@
         <v>89258111</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H69" s="1">
         <v>2</v>
@@ -5974,7 +5971,7 @@
         <v>29486020</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H70" s="1">
         <v>1</v>
@@ -6006,7 +6003,7 @@
         <v>30534151</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H71" s="1">
         <v>2</v>
@@ -6038,7 +6035,7 @@
         <v>40492520</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H72" s="1">
         <v>2</v>
@@ -6070,7 +6067,7 @@
         <v>40672045</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H73" s="1">
         <v>2</v>
@@ -6102,7 +6099,7 @@
         <v>46464032</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H74" s="1">
         <v>2</v>
@@ -6134,7 +6131,7 @@
         <v>49376026</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H75" s="1">
         <v>2</v>
@@ -6166,7 +6163,7 @@
         <v>73075459</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H76" s="1">
         <v>2</v>
@@ -6198,7 +6195,7 @@
         <v>98052346</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H77" s="1">
         <v>1</v>
@@ -6230,7 +6227,7 @@
         <v>15481084</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H78" s="1">
         <v>2</v>
@@ -6262,7 +6259,7 @@
         <v>39630579</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H79" s="1">
         <v>2</v>
@@ -6294,7 +6291,7 @@
         <v>83146202</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H80" s="1">
         <v>2</v>
@@ -6326,7 +6323,7 @@
         <v>86707179</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H81" s="1">
         <v>2</v>
@@ -6358,7 +6355,7 @@
         <v>40342542</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H82" s="1">
         <v>1</v>
@@ -6390,7 +6387,7 @@
         <v>78791420</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H83" s="1">
         <v>2</v>
@@ -6422,7 +6419,7 @@
         <v>1087</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H84" s="1">
         <v>2</v>
@@ -6454,7 +6451,7 @@
         <v>92040568</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H85" s="1">
         <v>2</v>
@@ -6486,7 +6483,7 @@
         <v>90</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H86" s="1">
         <v>2</v>
@@ -6518,7 +6515,7 @@
         <v>81700104</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H87" s="1">
         <v>1</v>
@@ -6550,7 +6547,7 @@
         <v>78771117</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H88" s="1">
         <v>2</v>
@@ -6582,7 +6579,7 @@
         <v>92</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H89" s="1">
         <v>2</v>
@@ -6614,7 +6611,7 @@
         <v>93</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H90" s="1">
         <v>2</v>
@@ -6646,7 +6643,7 @@
         <v>24460781</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H91" s="1">
         <v>1</v>
@@ -6678,7 +6675,7 @@
         <v>38447660</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H92" s="1">
         <v>2</v>
@@ -6710,7 +6707,7 @@
         <v>91</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H93" s="1">
         <v>2</v>
@@ -6742,7 +6739,7 @@
         <v>62104183</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H94" s="1">
         <v>2</v>
@@ -6774,7 +6771,7 @@
         <v>54709573</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H95" s="1">
         <v>2</v>
@@ -6806,7 +6803,7 @@
         <v>84352829</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H96" s="1">
         <v>2</v>
@@ -6838,7 +6835,7 @@
         <v>72641669</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H97" s="1">
         <v>1</v>
@@ -6870,7 +6867,7 @@
         <v>77424584</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H98" s="1">
         <v>2</v>
@@ -6902,7 +6899,7 @@
         <v>11627771</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H99" s="1">
         <v>2</v>
@@ -6934,7 +6931,7 @@
         <v>17389523</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H100" s="1">
         <v>2</v>
@@ -6966,7 +6963,7 @@
         <v>24800409</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>1088</v>
+        <v>6</v>
       </c>
       <c r="H101" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
upload page pulling data and changing content on frontend done
</commit_message>
<xml_diff>
--- a/database/Project_Data.xlsx
+++ b/database/Project_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffb\Desktop\Tecky\WSP\WSP012_Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6B703B-C5FC-4EFB-A184-8B82BF14D38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF66800-733B-4AFE-9FDE-44FBE25D14BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37" yWindow="10702" windowWidth="19394" windowHeight="11476" firstSheet="1" activeTab="2" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
   </bookViews>
@@ -3292,23 +3292,24 @@
     <t>sales_end_date</t>
   </si>
   <si>
+    <t>{"early_discount":false,"discount_amout":0,"early_date":null,"other_discount":{}}</t>
+  </si>
+  <si>
+    <t>2023-01-19 14:55:47</t>
+  </si>
+  <si>
+    <t>2023-01-18 14:55:47</t>
+  </si>
+  <si>
+    <t>38806715</t>
+  </si>
+  <si>
     <t>{
   "banner": "default_banner_picture.jpg",
   "title": "Default Title for the show",
+  "description":"A 100 Word description of your show",
   "content":"&lt;p&gt;&lt;strong&gt;Body&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;&lt;p&gt;Are you excited for the show?&lt;/p&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;&lt;p&gt;Show details:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;time&lt;/li&gt;&lt;li&gt;hello world&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.&lt;/p&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;"
 }</t>
-  </si>
-  <si>
-    <t>{"early_discount":false,"discount_amout":0,"early_date":null,"other_discount":{}}</t>
-  </si>
-  <si>
-    <t>2023-01-19 14:55:47</t>
-  </si>
-  <si>
-    <t>2023-01-18 14:55:47</t>
-  </si>
-  <si>
-    <t>38806715</t>
   </si>
 </sst>
 </file>
@@ -6416,7 +6417,7 @@
         <v>196</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>6</v>
@@ -8188,8 +8189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3255307-EFF8-4552-9330-483BB0071945}">
   <dimension ref="A1:N326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F59" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="E57" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8254,7 +8255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8268,10 +8269,10 @@
         <v>797</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F2" t="s">
         <v>1083</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1084</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -8298,7 +8299,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8312,10 +8313,10 @@
         <v>771</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F3" t="s">
         <v>1083</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1084</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -8342,7 +8343,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8356,10 +8357,10 @@
         <v>746</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F4" t="s">
         <v>1083</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1084</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -8386,7 +8387,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8400,10 +8401,10 @@
         <v>774</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F5" t="s">
         <v>1083</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1084</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -8430,7 +8431,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8444,10 +8445,10 @@
         <v>949</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F6" t="s">
         <v>1083</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1084</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -8474,7 +8475,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8488,10 +8489,10 @@
         <v>794</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F7" t="s">
         <v>1083</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1084</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -8518,7 +8519,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8532,10 +8533,10 @@
         <v>787</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F8" t="s">
         <v>1083</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1084</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -8562,7 +8563,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8576,10 +8577,10 @@
         <v>764</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F9" t="s">
         <v>1083</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1084</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -8606,7 +8607,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8620,10 +8621,10 @@
         <v>756</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F10" t="s">
         <v>1083</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1084</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -8650,7 +8651,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8664,10 +8665,10 @@
         <v>786</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F11" t="s">
         <v>1083</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1084</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -8694,7 +8695,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8708,10 +8709,10 @@
         <v>765</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F12" t="s">
         <v>1083</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1084</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -8738,7 +8739,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8752,10 +8753,10 @@
         <v>948</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F13" t="s">
         <v>1083</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1084</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -8782,7 +8783,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8796,10 +8797,10 @@
         <v>755</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F14" t="s">
         <v>1083</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1084</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -8826,7 +8827,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8840,10 +8841,10 @@
         <v>803</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F15" t="s">
         <v>1083</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1084</v>
       </c>
       <c r="G15">
         <v>4</v>
@@ -8870,7 +8871,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8884,10 +8885,10 @@
         <v>751</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F16" t="s">
         <v>1083</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1084</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -8914,7 +8915,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8928,10 +8929,10 @@
         <v>719</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F17" t="s">
         <v>1083</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1084</v>
       </c>
       <c r="G17">
         <v>4</v>
@@ -8958,7 +8959,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8972,10 +8973,10 @@
         <v>757</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F18" t="s">
         <v>1083</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1084</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -9002,7 +9003,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9016,10 +9017,10 @@
         <v>758</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F19" t="s">
         <v>1083</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1084</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -9046,7 +9047,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9060,10 +9061,10 @@
         <v>775</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F20" t="s">
         <v>1083</v>
-      </c>
-      <c r="F20" t="s">
-        <v>1084</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -9090,7 +9091,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9104,10 +9105,10 @@
         <v>795</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F21" t="s">
         <v>1083</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1084</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -9134,7 +9135,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9148,10 +9149,10 @@
         <v>759</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F22" t="s">
         <v>1083</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1084</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -9178,7 +9179,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9192,10 +9193,10 @@
         <v>766</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F23" t="s">
         <v>1083</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1084</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -9222,7 +9223,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9236,10 +9237,10 @@
         <v>767</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F24" t="s">
         <v>1083</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1084</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -9266,7 +9267,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9280,10 +9281,10 @@
         <v>788</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F25" t="s">
         <v>1083</v>
-      </c>
-      <c r="F25" t="s">
-        <v>1084</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -9310,7 +9311,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9324,10 +9325,10 @@
         <v>747</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F26" t="s">
         <v>1083</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1084</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -9354,7 +9355,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9368,10 +9369,10 @@
         <v>768</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F27" t="s">
         <v>1083</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1084</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -9398,7 +9399,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9412,10 +9413,10 @@
         <v>769</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F28" t="s">
         <v>1083</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1084</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -9442,7 +9443,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9456,10 +9457,10 @@
         <v>760</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F29" t="s">
         <v>1083</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1084</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -9486,7 +9487,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9500,10 +9501,10 @@
         <v>752</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F30" t="s">
         <v>1083</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1084</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -9530,7 +9531,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9544,10 +9545,10 @@
         <v>720</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F31" t="s">
         <v>1083</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1084</v>
       </c>
       <c r="G31">
         <v>4</v>
@@ -9574,7 +9575,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9588,10 +9589,10 @@
         <v>798</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F32" t="s">
         <v>1083</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1084</v>
       </c>
       <c r="G32">
         <v>2</v>
@@ -9618,7 +9619,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9632,10 +9633,10 @@
         <v>770</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F33" t="s">
         <v>1083</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1084</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -9662,7 +9663,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9676,10 +9677,10 @@
         <v>796</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F34" t="s">
         <v>1083</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1084</v>
       </c>
       <c r="G34">
         <v>2</v>
@@ -9706,7 +9707,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9720,10 +9721,10 @@
         <v>761</v>
       </c>
       <c r="E35" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F35" t="s">
         <v>1083</v>
-      </c>
-      <c r="F35" t="s">
-        <v>1084</v>
       </c>
       <c r="G35">
         <v>2</v>
@@ -9750,7 +9751,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9764,10 +9765,10 @@
         <v>748</v>
       </c>
       <c r="E36" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F36" t="s">
         <v>1083</v>
-      </c>
-      <c r="F36" t="s">
-        <v>1084</v>
       </c>
       <c r="G36">
         <v>2</v>
@@ -9794,7 +9795,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9808,10 +9809,10 @@
         <v>776</v>
       </c>
       <c r="E37" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F37" t="s">
         <v>1083</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1084</v>
       </c>
       <c r="G37">
         <v>4</v>
@@ -9838,7 +9839,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9852,10 +9853,10 @@
         <v>754</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F38" t="s">
         <v>1083</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1084</v>
       </c>
       <c r="G38">
         <v>2</v>
@@ -9882,7 +9883,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9896,10 +9897,10 @@
         <v>722</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F39" t="s">
         <v>1083</v>
-      </c>
-      <c r="F39" t="s">
-        <v>1084</v>
       </c>
       <c r="G39">
         <v>4</v>
@@ -9926,7 +9927,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9940,10 +9941,10 @@
         <v>799</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F40" t="s">
         <v>1083</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1084</v>
       </c>
       <c r="G40">
         <v>2</v>
@@ -9970,7 +9971,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9984,10 +9985,10 @@
         <v>789</v>
       </c>
       <c r="E41" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F41" t="s">
         <v>1083</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1084</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -10014,7 +10015,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10028,10 +10029,10 @@
         <v>755</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F42" t="s">
         <v>1083</v>
-      </c>
-      <c r="F42" t="s">
-        <v>1084</v>
       </c>
       <c r="G42">
         <v>2</v>
@@ -10058,7 +10059,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10072,10 +10073,10 @@
         <v>790</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F43" t="s">
         <v>1083</v>
-      </c>
-      <c r="F43" t="s">
-        <v>1084</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -10102,7 +10103,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10116,10 +10117,10 @@
         <v>800</v>
       </c>
       <c r="E44" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F44" t="s">
         <v>1083</v>
-      </c>
-      <c r="F44" t="s">
-        <v>1084</v>
       </c>
       <c r="G44">
         <v>2</v>
@@ -10146,7 +10147,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10160,10 +10161,10 @@
         <v>804</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F45" t="s">
         <v>1083</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1084</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -10190,7 +10191,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10204,10 +10205,10 @@
         <v>801</v>
       </c>
       <c r="E46" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F46" t="s">
         <v>1083</v>
-      </c>
-      <c r="F46" t="s">
-        <v>1084</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -10234,7 +10235,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -10248,10 +10249,10 @@
         <v>749</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F47" t="s">
         <v>1083</v>
-      </c>
-      <c r="F47" t="s">
-        <v>1084</v>
       </c>
       <c r="G47">
         <v>2</v>
@@ -10278,7 +10279,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -10292,10 +10293,10 @@
         <v>750</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F48" t="s">
         <v>1083</v>
-      </c>
-      <c r="F48" t="s">
-        <v>1084</v>
       </c>
       <c r="G48">
         <v>2</v>
@@ -10322,7 +10323,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -10336,10 +10337,10 @@
         <v>773</v>
       </c>
       <c r="E49" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F49" t="s">
         <v>1083</v>
-      </c>
-      <c r="F49" t="s">
-        <v>1084</v>
       </c>
       <c r="G49">
         <v>4</v>
@@ -10366,7 +10367,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -10380,10 +10381,10 @@
         <v>762</v>
       </c>
       <c r="E50" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F50" t="s">
         <v>1083</v>
-      </c>
-      <c r="F50" t="s">
-        <v>1084</v>
       </c>
       <c r="G50">
         <v>2</v>
@@ -10410,7 +10411,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51</v>
       </c>
@@ -10424,10 +10425,10 @@
         <v>721</v>
       </c>
       <c r="E51" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F51" t="s">
         <v>1083</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1084</v>
       </c>
       <c r="G51">
         <v>4</v>
@@ -10454,7 +10455,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
@@ -10468,10 +10469,10 @@
         <v>753</v>
       </c>
       <c r="E52" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F52" t="s">
         <v>1083</v>
-      </c>
-      <c r="F52" t="s">
-        <v>1084</v>
       </c>
       <c r="G52">
         <v>2</v>
@@ -10498,7 +10499,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -10512,10 +10513,10 @@
         <v>777</v>
       </c>
       <c r="E53" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F53" t="s">
         <v>1083</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1084</v>
       </c>
       <c r="G53">
         <v>4</v>
@@ -10542,7 +10543,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -10556,10 +10557,10 @@
         <v>758</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F54" t="s">
         <v>1083</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1084</v>
       </c>
       <c r="G54">
         <v>2</v>
@@ -10586,7 +10587,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -10600,10 +10601,10 @@
         <v>782</v>
       </c>
       <c r="E55" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F55" t="s">
         <v>1083</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1084</v>
       </c>
       <c r="G55">
         <v>4</v>
@@ -10630,7 +10631,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>56</v>
       </c>
@@ -10644,10 +10645,10 @@
         <v>763</v>
       </c>
       <c r="E56" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F56" t="s">
         <v>1083</v>
-      </c>
-      <c r="F56" t="s">
-        <v>1084</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -10674,7 +10675,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>57</v>
       </c>
@@ -10688,10 +10689,10 @@
         <v>802</v>
       </c>
       <c r="E57" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F57" t="s">
         <v>1083</v>
-      </c>
-      <c r="F57" t="s">
-        <v>1084</v>
       </c>
       <c r="G57">
         <v>2</v>
@@ -10718,7 +10719,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
@@ -10732,10 +10733,10 @@
         <v>778</v>
       </c>
       <c r="E58" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F58" t="s">
         <v>1083</v>
-      </c>
-      <c r="F58" t="s">
-        <v>1084</v>
       </c>
       <c r="G58">
         <v>4</v>
@@ -10762,7 +10763,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
@@ -10776,10 +10777,10 @@
         <v>772</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F59" t="s">
         <v>1083</v>
-      </c>
-      <c r="F59" t="s">
-        <v>1084</v>
       </c>
       <c r="G59">
         <v>4</v>
@@ -13525,10 +13526,10 @@
         <v>1079</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -13539,10 +13540,10 @@
         <v>956</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
header nav bar and template css complete
</commit_message>
<xml_diff>
--- a/database/Project_Data.xlsx
+++ b/database/Project_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffb\Desktop\Tecky\WSP\WSP012_Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F99AE4B-35DC-4D24-83C0-7990527BE146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F796A3-72F9-4FED-A71E-07B0E47D604F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="11" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{92F08B71-07A5-45B0-99A1-9C8247BDFA47}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3512" uniqueCount="1088">
   <si>
     <t>id</t>
   </si>
@@ -3307,6 +3307,9 @@
   </si>
   <si>
     <t>[pending]</t>
+  </si>
+  <si>
+    <t>default_icon.png</t>
   </si>
 </sst>
 </file>
@@ -3722,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89681126-5237-455A-856C-2B26CBD7FB95}">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,6 +3796,9 @@
       <c r="E2" s="1">
         <v>24525402</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3825,6 +3831,9 @@
       <c r="E3" s="1">
         <v>57060794</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3857,6 +3866,9 @@
       <c r="E4" s="1">
         <v>94713906</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3889,6 +3901,9 @@
       <c r="E5" s="1">
         <v>14685757</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
@@ -3921,6 +3936,9 @@
       <c r="E6" s="1">
         <v>60515705</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3953,6 +3971,9 @@
       <c r="E7" s="1">
         <v>28207629</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
@@ -3985,6 +4006,9 @@
       <c r="E8" s="1">
         <v>52947240</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
@@ -4017,6 +4041,9 @@
       <c r="E9" s="1">
         <v>34170541</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4049,6 +4076,9 @@
       <c r="E10" s="1">
         <v>82903004</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4081,6 +4111,9 @@
       <c r="E11" s="1">
         <v>60303237</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
@@ -4113,6 +4146,9 @@
       <c r="E12" s="1">
         <v>36493531</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
@@ -4145,6 +4181,9 @@
       <c r="E13" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>6</v>
       </c>
@@ -4177,6 +4216,9 @@
       <c r="E14" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
@@ -4209,6 +4251,9 @@
       <c r="E15" s="1">
         <v>46626259</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
@@ -4241,6 +4286,9 @@
       <c r="E16" s="1">
         <v>14903335</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>6</v>
       </c>
@@ -4273,6 +4321,9 @@
       <c r="E17" s="1">
         <v>86583052</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>6</v>
       </c>
@@ -4305,6 +4356,9 @@
       <c r="E18" s="1">
         <v>69011866</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>6</v>
       </c>
@@ -4337,6 +4391,9 @@
       <c r="E19" s="1">
         <v>86467584</v>
       </c>
+      <c r="F19" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>6</v>
       </c>
@@ -4369,6 +4426,9 @@
       <c r="E20" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="F20" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G20" s="1" t="s">
         <v>6</v>
       </c>
@@ -4401,6 +4461,9 @@
       <c r="E21" s="1">
         <v>38142143</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>6</v>
       </c>
@@ -4433,6 +4496,9 @@
       <c r="E22" s="1">
         <v>62084515</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>6</v>
       </c>
@@ -4465,6 +4531,9 @@
       <c r="E23" s="1">
         <v>25890369</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>6</v>
       </c>
@@ -4497,6 +4566,9 @@
       <c r="E24" s="1">
         <v>10223266</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>6</v>
       </c>
@@ -4529,6 +4601,9 @@
       <c r="E25" s="1">
         <v>21984532</v>
       </c>
+      <c r="F25" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>6</v>
       </c>
@@ -4561,6 +4636,9 @@
       <c r="E26" s="1">
         <v>37299097</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>6</v>
       </c>
@@ -4593,6 +4671,9 @@
       <c r="E27" s="1">
         <v>42689302</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G27" s="1" t="s">
         <v>6</v>
       </c>
@@ -4625,6 +4706,9 @@
       <c r="E28" s="1">
         <v>92825467</v>
       </c>
+      <c r="F28" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G28" s="1" t="s">
         <v>6</v>
       </c>
@@ -4657,6 +4741,9 @@
       <c r="E29" s="1">
         <v>59809431</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>6</v>
       </c>
@@ -4689,6 +4776,9 @@
       <c r="E30" s="1">
         <v>90994799</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>6</v>
       </c>
@@ -4721,6 +4811,9 @@
       <c r="E31" s="1">
         <v>92235387</v>
       </c>
+      <c r="F31" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>6</v>
       </c>
@@ -4753,6 +4846,9 @@
       <c r="E32" s="1">
         <v>79262859</v>
       </c>
+      <c r="F32" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G32" s="1" t="s">
         <v>6</v>
       </c>
@@ -4785,6 +4881,9 @@
       <c r="E33" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="F33" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G33" s="1" t="s">
         <v>6</v>
       </c>
@@ -4817,6 +4916,9 @@
       <c r="E34" s="1">
         <v>26434632</v>
       </c>
+      <c r="F34" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>6</v>
       </c>
@@ -4849,6 +4951,9 @@
       <c r="E35" s="1">
         <v>78887454</v>
       </c>
+      <c r="F35" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>6</v>
       </c>
@@ -4881,6 +4986,9 @@
       <c r="E36" s="1">
         <v>72440777</v>
       </c>
+      <c r="F36" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>6</v>
       </c>
@@ -4913,6 +5021,9 @@
       <c r="E37" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="F37" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>6</v>
       </c>
@@ -4945,6 +5056,9 @@
       <c r="E38" s="1">
         <v>19091891</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G38" s="1" t="s">
         <v>6</v>
       </c>
@@ -4977,6 +5091,9 @@
       <c r="E39" s="1">
         <v>90557839</v>
       </c>
+      <c r="F39" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G39" s="1" t="s">
         <v>6</v>
       </c>
@@ -5009,6 +5126,9 @@
       <c r="E40" s="1">
         <v>68043701</v>
       </c>
+      <c r="F40" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G40" s="1" t="s">
         <v>6</v>
       </c>
@@ -5041,6 +5161,9 @@
       <c r="E41" s="1">
         <v>42426903</v>
       </c>
+      <c r="F41" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>6</v>
       </c>
@@ -5073,6 +5196,9 @@
       <c r="E42" s="1">
         <v>46681742</v>
       </c>
+      <c r="F42" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G42" s="1" t="s">
         <v>6</v>
       </c>
@@ -5105,6 +5231,9 @@
       <c r="E43" s="1">
         <v>93975858</v>
       </c>
+      <c r="F43" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>6</v>
       </c>
@@ -5137,6 +5266,9 @@
       <c r="E44" s="1">
         <v>35188903</v>
       </c>
+      <c r="F44" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>6</v>
       </c>
@@ -5169,6 +5301,9 @@
       <c r="E45" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>6</v>
       </c>
@@ -5201,6 +5336,9 @@
       <c r="E46" s="1">
         <v>28729013</v>
       </c>
+      <c r="F46" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>6</v>
       </c>
@@ -5233,6 +5371,9 @@
       <c r="E47" s="1">
         <v>22570600</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G47" s="1" t="s">
         <v>6</v>
       </c>
@@ -5265,6 +5406,9 @@
       <c r="E48" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="F48" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G48" s="1" t="s">
         <v>6</v>
       </c>
@@ -5297,6 +5441,9 @@
       <c r="E49" s="1">
         <v>86922958</v>
       </c>
+      <c r="F49" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G49" s="1" t="s">
         <v>6</v>
       </c>
@@ -5329,6 +5476,9 @@
       <c r="E50" s="1">
         <v>86436566</v>
       </c>
+      <c r="F50" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G50" s="1" t="s">
         <v>6</v>
       </c>
@@ -5361,6 +5511,9 @@
       <c r="E51" s="1">
         <v>75380206</v>
       </c>
+      <c r="F51" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G51" s="1" t="s">
         <v>6</v>
       </c>
@@ -5393,6 +5546,9 @@
       <c r="E52" s="1">
         <v>18270909</v>
       </c>
+      <c r="F52" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G52" s="1" t="s">
         <v>6</v>
       </c>
@@ -5425,6 +5581,9 @@
       <c r="E53" s="1">
         <v>62564319</v>
       </c>
+      <c r="F53" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>6</v>
       </c>
@@ -5457,6 +5616,9 @@
       <c r="E54" s="1">
         <v>73182935</v>
       </c>
+      <c r="F54" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>6</v>
       </c>
@@ -5489,6 +5651,9 @@
       <c r="E55" s="1">
         <v>21770892</v>
       </c>
+      <c r="F55" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G55" s="1" t="s">
         <v>6</v>
       </c>
@@ -5521,6 +5686,9 @@
       <c r="E56" s="1">
         <v>89032776</v>
       </c>
+      <c r="F56" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G56" s="1" t="s">
         <v>6</v>
       </c>
@@ -5553,6 +5721,9 @@
       <c r="E57" s="1">
         <v>84401453</v>
       </c>
+      <c r="F57" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G57" s="1" t="s">
         <v>6</v>
       </c>
@@ -5585,6 +5756,9 @@
       <c r="E58" s="1">
         <v>34287307</v>
       </c>
+      <c r="F58" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G58" s="1" t="s">
         <v>6</v>
       </c>
@@ -5617,6 +5791,9 @@
       <c r="E59" s="1">
         <v>18713246</v>
       </c>
+      <c r="F59" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G59" s="1" t="s">
         <v>6</v>
       </c>
@@ -5649,6 +5826,9 @@
       <c r="E60" s="1">
         <v>55298168</v>
       </c>
+      <c r="F60" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G60" s="1" t="s">
         <v>6</v>
       </c>
@@ -5681,6 +5861,9 @@
       <c r="E61" s="1">
         <v>31430907</v>
       </c>
+      <c r="F61" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>6</v>
       </c>
@@ -5713,6 +5896,9 @@
       <c r="E62" s="1">
         <v>47024498</v>
       </c>
+      <c r="F62" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G62" s="1" t="s">
         <v>6</v>
       </c>
@@ -5745,6 +5931,9 @@
       <c r="E63" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="F63" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G63" s="1" t="s">
         <v>6</v>
       </c>
@@ -5777,6 +5966,9 @@
       <c r="E64" s="1">
         <v>17040135</v>
       </c>
+      <c r="F64" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>6</v>
       </c>
@@ -5809,6 +6001,9 @@
       <c r="E65" s="1">
         <v>68540910</v>
       </c>
+      <c r="F65" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G65" s="1" t="s">
         <v>6</v>
       </c>
@@ -5841,6 +6036,9 @@
       <c r="E66" s="1">
         <v>80325877</v>
       </c>
+      <c r="F66" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G66" s="1" t="s">
         <v>6</v>
       </c>
@@ -5873,6 +6071,9 @@
       <c r="E67" s="1">
         <v>67307935</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G67" s="1" t="s">
         <v>6</v>
       </c>
@@ -5905,6 +6106,9 @@
       <c r="E68" s="1">
         <v>19534338</v>
       </c>
+      <c r="F68" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G68" s="1" t="s">
         <v>6</v>
       </c>
@@ -5937,6 +6141,9 @@
       <c r="E69" s="1">
         <v>89258111</v>
       </c>
+      <c r="F69" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G69" s="1" t="s">
         <v>6</v>
       </c>
@@ -5969,6 +6176,9 @@
       <c r="E70" s="1">
         <v>29486020</v>
       </c>
+      <c r="F70" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G70" s="1" t="s">
         <v>6</v>
       </c>
@@ -6001,6 +6211,9 @@
       <c r="E71" s="1">
         <v>30534151</v>
       </c>
+      <c r="F71" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>6</v>
       </c>
@@ -6033,6 +6246,9 @@
       <c r="E72" s="1">
         <v>40492520</v>
       </c>
+      <c r="F72" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G72" s="1" t="s">
         <v>6</v>
       </c>
@@ -6065,6 +6281,9 @@
       <c r="E73" s="1">
         <v>40672045</v>
       </c>
+      <c r="F73" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G73" s="1" t="s">
         <v>6</v>
       </c>
@@ -6097,6 +6316,9 @@
       <c r="E74" s="1">
         <v>46464032</v>
       </c>
+      <c r="F74" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G74" s="1" t="s">
         <v>6</v>
       </c>
@@ -6129,6 +6351,9 @@
       <c r="E75" s="1">
         <v>49376026</v>
       </c>
+      <c r="F75" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G75" s="1" t="s">
         <v>6</v>
       </c>
@@ -6161,6 +6386,9 @@
       <c r="E76" s="1">
         <v>73075459</v>
       </c>
+      <c r="F76" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>6</v>
       </c>
@@ -6193,6 +6421,9 @@
       <c r="E77" s="1">
         <v>98052346</v>
       </c>
+      <c r="F77" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G77" s="1" t="s">
         <v>6</v>
       </c>
@@ -6225,6 +6456,9 @@
       <c r="E78" s="1">
         <v>15481084</v>
       </c>
+      <c r="F78" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G78" s="1" t="s">
         <v>6</v>
       </c>
@@ -6257,6 +6491,9 @@
       <c r="E79" s="1">
         <v>39630579</v>
       </c>
+      <c r="F79" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G79" s="1" t="s">
         <v>6</v>
       </c>
@@ -6289,6 +6526,9 @@
       <c r="E80" s="1">
         <v>83146202</v>
       </c>
+      <c r="F80" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G80" s="1" t="s">
         <v>6</v>
       </c>
@@ -6321,6 +6561,9 @@
       <c r="E81" s="1">
         <v>86707179</v>
       </c>
+      <c r="F81" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G81" s="1" t="s">
         <v>6</v>
       </c>
@@ -6353,6 +6596,9 @@
       <c r="E82" s="1">
         <v>40342542</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G82" s="1" t="s">
         <v>6</v>
       </c>
@@ -6385,6 +6631,9 @@
       <c r="E83" s="1">
         <v>78791420</v>
       </c>
+      <c r="F83" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G83" s="1" t="s">
         <v>6</v>
       </c>
@@ -6417,6 +6666,9 @@
       <c r="E84" s="1" t="s">
         <v>1084</v>
       </c>
+      <c r="F84" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G84" s="1" t="s">
         <v>6</v>
       </c>
@@ -6449,6 +6701,9 @@
       <c r="E85" s="1">
         <v>92040568</v>
       </c>
+      <c r="F85" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>6</v>
       </c>
@@ -6481,6 +6736,9 @@
       <c r="E86" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="F86" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G86" s="1" t="s">
         <v>6</v>
       </c>
@@ -6513,6 +6771,9 @@
       <c r="E87" s="1">
         <v>81700104</v>
       </c>
+      <c r="F87" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G87" s="1" t="s">
         <v>6</v>
       </c>
@@ -6545,6 +6806,9 @@
       <c r="E88" s="1">
         <v>78771117</v>
       </c>
+      <c r="F88" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G88" s="1" t="s">
         <v>6</v>
       </c>
@@ -6577,6 +6841,9 @@
       <c r="E89" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="F89" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G89" s="1" t="s">
         <v>6</v>
       </c>
@@ -6609,6 +6876,9 @@
       <c r="E90" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="F90" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G90" s="1" t="s">
         <v>6</v>
       </c>
@@ -6641,6 +6911,9 @@
       <c r="E91" s="1">
         <v>24460781</v>
       </c>
+      <c r="F91" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G91" s="1" t="s">
         <v>6</v>
       </c>
@@ -6673,6 +6946,9 @@
       <c r="E92" s="1">
         <v>38447660</v>
       </c>
+      <c r="F92" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G92" s="1" t="s">
         <v>6</v>
       </c>
@@ -6705,6 +6981,9 @@
       <c r="E93" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="F93" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G93" s="1" t="s">
         <v>6</v>
       </c>
@@ -6737,6 +7016,9 @@
       <c r="E94" s="1">
         <v>62104183</v>
       </c>
+      <c r="F94" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G94" s="1" t="s">
         <v>6</v>
       </c>
@@ -6769,6 +7051,9 @@
       <c r="E95" s="1">
         <v>54709573</v>
       </c>
+      <c r="F95" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G95" s="1" t="s">
         <v>6</v>
       </c>
@@ -6801,6 +7086,9 @@
       <c r="E96" s="1">
         <v>84352829</v>
       </c>
+      <c r="F96" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G96" s="1" t="s">
         <v>6</v>
       </c>
@@ -6833,6 +7121,9 @@
       <c r="E97" s="1">
         <v>72641669</v>
       </c>
+      <c r="F97" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G97" s="1" t="s">
         <v>6</v>
       </c>
@@ -6865,6 +7156,9 @@
       <c r="E98" s="1">
         <v>77424584</v>
       </c>
+      <c r="F98" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G98" s="1" t="s">
         <v>6</v>
       </c>
@@ -6897,6 +7191,9 @@
       <c r="E99" s="1">
         <v>11627771</v>
       </c>
+      <c r="F99" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G99" s="1" t="s">
         <v>6</v>
       </c>
@@ -6929,6 +7226,9 @@
       <c r="E100" s="1">
         <v>17389523</v>
       </c>
+      <c r="F100" s="1" t="s">
+        <v>1087</v>
+      </c>
       <c r="G100" s="1" t="s">
         <v>6</v>
       </c>
@@ -6960,6 +7260,9 @@
       </c>
       <c r="E101" s="1">
         <v>24800409</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>1087</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>6</v>
@@ -8221,7 +8524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C415E28E-75D8-4383-BA14-825E63676B6A}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>

</xml_diff>